<commit_message>
Source for layer definition
</commit_message>
<xml_diff>
--- a/mmowgli2/src/edu/nps/moves/mmowgli/modules/maps/LeafletLayers.xlsx
+++ b/mmowgli2/src/edu/nps/moves/mmowgli/modules/maps/LeafletLayers.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="660" yWindow="240" windowWidth="37620" windowHeight="17060" tabRatio="500"/>
+    <workbookView xWindow="6660" yWindow="2900" windowWidth="37620" windowHeight="17060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -851,8 +851,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N34"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="F23" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1658,6 +1658,9 @@
       <c r="F33" s="4" t="s">
         <v>104</v>
       </c>
+      <c r="H33">
+        <v>0.25</v>
+      </c>
       <c r="J33" t="b">
         <v>1</v>
       </c>
@@ -1686,6 +1689,9 @@
       </c>
       <c r="F34" s="4" t="s">
         <v>104</v>
+      </c>
+      <c r="H34">
+        <v>0.25</v>
       </c>
       <c r="J34" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
Control leaflet layers persistently
</commit_message>
<xml_diff>
--- a/mmowgli2/src/edu/nps/moves/mmowgli/modules/maps/LeafletLayers.xlsx
+++ b/mmowgli2/src/edu/nps/moves/mmowgli/modules/maps/LeafletLayers.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6660" yWindow="2940" windowWidth="37620" windowHeight="17060" tabRatio="500"/>
+    <workbookView xWindow="5700" yWindow="9740" windowWidth="37620" windowHeight="17060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -861,7 +861,7 @@
   <dimension ref="A1:N34"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -934,6 +934,9 @@
       <c r="C2" t="b">
         <v>1</v>
       </c>
+      <c r="D2" t="b">
+        <v>1</v>
+      </c>
       <c r="E2" t="s">
         <v>51</v>
       </c>
@@ -1121,9 +1124,6 @@
         <v>31</v>
       </c>
       <c r="C9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D9" t="b">
         <v>1</v>
       </c>
       <c r="E9" t="s">

</xml_diff>